<commit_message>
Adding, editing, deleting Products and Artists
</commit_message>
<xml_diff>
--- a/AppClasses/ProductTestImport.xlsx
+++ b/AppClasses/ProductTestImport.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,10 +427,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>4324</v>
+        <v>14</v>
       </c>
       <c r="B4">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>

</xml_diff>